<commit_message>
support for n_blank_allowed param to TabularIo.load
</commit_message>
<xml_diff>
--- a/test/dummy/test/input/correct_xlsx.xlsx
+++ b/test/dummy/test/input/correct_xlsx.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10917"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11127"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/eric/Repos/lycensed/test/data/sheets/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/eric/Repos/terrier-engine/test/dummy/test/input/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{25061FB0-48F4-4F4D-B736-F8BB6F9C0B31}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2EB23526-90E7-5243-8F65-FF5A2426B100}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1700" yWindow="1540" windowWidth="28040" windowHeight="17440" xr2:uid="{AD3F18AD-AB10-6B40-9EAA-789A0C8696F2}"/>
+    <workbookView xWindow="7440" yWindow="1180" windowWidth="28040" windowHeight="17440" xr2:uid="{AD3F18AD-AB10-6B40-9EAA-789A0C8696F2}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -434,10 +434,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F918C6C0-A062-5F40-A29D-E70DDE9F15B0}">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="A2:D3"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -475,24 +475,24 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A3" s="1" t="s">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B4" t="s">
         <v>9</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C4" t="s">
         <v>10</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D4" t="s">
         <v>11</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="A2" r:id="rId1" xr:uid="{AAD4BEDC-2CE8-C74E-A2CA-DD25B3D46C8C}"/>
-    <hyperlink ref="A3" r:id="rId2" xr:uid="{0EF9616A-436A-544B-B23A-DEC936078D01}"/>
+    <hyperlink ref="A4" r:id="rId2" xr:uid="{0EF9616A-436A-544B-B23A-DEC936078D01}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>